<commit_message>
change excel format in bulk invoicing of sales main and merge
</commit_message>
<xml_diff>
--- a/uploads/excel/bulk_upload_sales_main.xlsx
+++ b/uploads/excel/bulk_upload_sales_main.xlsx
@@ -52,9 +52,6 @@
     <t>Invoice Number</t>
   </si>
   <si>
-    <t>Actual Billing ID</t>
-  </si>
-  <si>
     <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                               </t>
   </si>
   <si>
@@ -67,10 +64,13 @@
     <t>1590EC_SS</t>
   </si>
   <si>
-    <t>ACERES</t>
-  </si>
-  <si>
-    <t>ACENGES</t>
+    <t>Settlement ID</t>
+  </si>
+  <si>
+    <t>ABRECO</t>
+  </si>
+  <si>
+    <t>ABSOLUTDI</t>
   </si>
 </sst>
 </file>
@@ -95,29 +95,23 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF444444"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -136,10 +130,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,22 +449,22 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -485,13 +477,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3">
         <v>1001</v>
       </c>
       <c r="G2" t="s">
@@ -499,46 +491,46 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3">
         <v>1002</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>1003</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>1004</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>